<commit_message>
Progresso dos experimentos (agora faltam aproximadamente 10 dias para finalizar os experimentos).
</commit_message>
<xml_diff>
--- a/PaperNeural/Results/ResultsMar2017-t-SNE_MI_1000_LR_400_PE_16.xlsx
+++ b/PaperNeural/Results/ResultsMar2017-t-SNE_MI_1000_LR_400_PE_16.xlsx
@@ -11589,34 +11589,56 @@
       <c r="B24" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="C24" s="40"/>
-      <c r="D24" s="40"/>
-      <c r="E24" s="40"/>
+      <c r="C24" s="40" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="D24" s="40" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="E24" s="40" t="n">
+        <v>0.0</v>
+      </c>
       <c r="F24" s="3" t="e">
         <f>100*C24/SUM(C24:E24)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="G24" s="63"/>
+      <c r="G24" s="63" t="n">
+        <v>15.789473684210526</v>
+      </c>
       <c r="I24" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="J24" s="40"/>
-      <c r="K24" s="40"/>
-      <c r="L24" s="40"/>
+      <c r="J24" s="40" t="n">
+        <v>0.9555555555555556</v>
+      </c>
+      <c r="K24" s="40" t="n">
+        <v>0.022222222222222223</v>
+      </c>
+      <c r="L24" s="40" t="n">
+        <v>0.022222222222222223</v>
+      </c>
       <c r="M24" s="3" t="e">
         <f>100*J24/(SUM(J24:L24))</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="N24" s="63"/>
+      <c r="N24" s="63" t="n">
+        <v>3.508771929824561</v>
+      </c>
     </row>
     <row r="25" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A25" s="61"/>
       <c r="B25" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="C25" s="40"/>
-      <c r="D25" s="40"/>
-      <c r="E25" s="40"/>
+      <c r="C25" s="40" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D25" s="40" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="E25" s="40" t="n">
+        <v>0.25</v>
+      </c>
       <c r="F25" s="3" t="e">
         <f>100*D25/SUM(C25:E25)</f>
         <v>#DIV/0!</v>
@@ -11625,9 +11647,15 @@
       <c r="I25" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="J25" s="40"/>
-      <c r="K25" s="40"/>
-      <c r="L25" s="40"/>
+      <c r="J25" s="40" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="K25" s="40" t="n">
+        <v>0.9861111111111112</v>
+      </c>
+      <c r="L25" s="40" t="n">
+        <v>0.013888888888888888</v>
+      </c>
       <c r="M25" s="3" t="e">
         <f>100*K25/(SUM(J25:L25))</f>
         <v>#DIV/0!</v>
@@ -11639,9 +11667,15 @@
       <c r="B26" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="C26" s="40"/>
-      <c r="D26" s="40"/>
-      <c r="E26" s="40"/>
+      <c r="C26" s="40" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D26" s="40" t="n">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="E26" s="40" t="n">
+        <v>0.8333333333333334</v>
+      </c>
       <c r="F26" s="3" t="e">
         <f>100*E26/SUM(C26:E26)</f>
         <v>#DIV/0!</v>
@@ -11650,9 +11684,15 @@
       <c r="I26" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="J26" s="40"/>
-      <c r="K26" s="40"/>
-      <c r="L26" s="40"/>
+      <c r="J26" s="40" t="n">
+        <v>0.018518518518518517</v>
+      </c>
+      <c r="K26" s="40" t="n">
+        <v>0.037037037037037035</v>
+      </c>
+      <c r="L26" s="40" t="n">
+        <v>0.9444444444444444</v>
+      </c>
       <c r="M26" s="3" t="e">
         <f>100*L26/(SUM(J26:L26))</f>
         <v>#DIV/0!</v>
@@ -12349,34 +12389,56 @@
       <c r="B24" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="C24" s="40"/>
-      <c r="D24" s="40"/>
-      <c r="E24" s="40"/>
+      <c r="C24" s="40" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="D24" s="40" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="E24" s="40" t="n">
+        <v>0.0</v>
+      </c>
       <c r="F24" s="3" t="e">
         <f>100*C24/SUM(C24:E24)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="G24" s="63"/>
+      <c r="G24" s="63" t="n">
+        <v>31.57894736842105</v>
+      </c>
       <c r="I24" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="J24" s="40"/>
-      <c r="K24" s="40"/>
-      <c r="L24" s="40"/>
+      <c r="J24" s="40" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="K24" s="40" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L24" s="40" t="n">
+        <v>0.0</v>
+      </c>
       <c r="M24" s="3" t="e">
         <f>100*J24/(SUM(J24:L24))</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="N24" s="63"/>
+      <c r="N24" s="63" t="n">
+        <v>4.093567251461988</v>
+      </c>
     </row>
     <row r="25" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A25" s="61"/>
       <c r="B25" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="C25" s="40"/>
-      <c r="D25" s="40"/>
-      <c r="E25" s="40"/>
+      <c r="C25" s="40" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D25" s="40" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="E25" s="40" t="n">
+        <v>0.25</v>
+      </c>
       <c r="F25" s="3" t="e">
         <f>100*D25/SUM(C25:E25)</f>
         <v>#DIV/0!</v>
@@ -12385,9 +12447,15 @@
       <c r="I25" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="J25" s="40"/>
-      <c r="K25" s="40"/>
-      <c r="L25" s="40"/>
+      <c r="J25" s="40" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="K25" s="40" t="n">
+        <v>0.9722222222222222</v>
+      </c>
+      <c r="L25" s="40" t="n">
+        <v>0.027777777777777776</v>
+      </c>
       <c r="M25" s="3" t="e">
         <f>100*K25/(SUM(J25:L25))</f>
         <v>#DIV/0!</v>
@@ -12399,9 +12467,15 @@
       <c r="B26" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="C26" s="40"/>
-      <c r="D26" s="40"/>
-      <c r="E26" s="40"/>
+      <c r="C26" s="40" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D26" s="40" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="E26" s="40" t="n">
+        <v>0.5</v>
+      </c>
       <c r="F26" s="3" t="e">
         <f>100*E26/SUM(C26:E26)</f>
         <v>#DIV/0!</v>
@@ -12410,9 +12484,15 @@
       <c r="I26" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="J26" s="40"/>
-      <c r="K26" s="40"/>
-      <c r="L26" s="40"/>
+      <c r="J26" s="40" t="n">
+        <v>0.037037037037037035</v>
+      </c>
+      <c r="K26" s="40" t="n">
+        <v>0.05555555555555555</v>
+      </c>
+      <c r="L26" s="40" t="n">
+        <v>0.9074074074074074</v>
+      </c>
       <c r="M26" s="3" t="e">
         <f>100*L26/(SUM(J26:L26))</f>
         <v>#DIV/0!</v>

</xml_diff>